<commit_message>
Notas corrigidas Paula Regufe
</commit_message>
<xml_diff>
--- a/dados/psico/notasProvas.xlsx
+++ b/dados/psico/notasProvas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gilberto\OneDrive\Documentos\1sem2016\psicologia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gilberto\OneDrive\Documentos\pagina\gpsassi.github.io\dados\psico\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1944,13 +1944,16 @@
       <c r="G43">
         <v>1</v>
       </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
       <c r="I43">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J43">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2492,7 +2495,7 @@
       </c>
       <c r="J61" s="3">
         <f>AVERAGE(J2:J59)</f>
-        <v>6.7758620689655151</v>
+        <v>6.7931034482758603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
notas autualizadas da psicologia
</commit_message>
<xml_diff>
--- a/dados/psico/notasProvas.xlsx
+++ b/dados/psico/notasProvas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gilberto\OneDrive\Documentos\pagina\gpsassi.github.io\dados\psico\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gilberto\OneDrive\Documentos\1sem2016\psicologia\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1849,13 +1849,16 @@
       <c r="G40">
         <v>1</v>
       </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J40">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2498,7 +2501,7 @@
       </c>
       <c r="J61" s="3">
         <f>AVERAGE(J2:J59)</f>
-        <v>6.8318965517241361</v>
+        <v>6.8491379310344804</v>
       </c>
     </row>
   </sheetData>

</xml_diff>